<commit_message>
Update reglas de nomina
</commit_message>
<xml_diff>
--- a/reglas-nomina.xlsx
+++ b/reglas-nomina.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Nombre</t>
   </si>
@@ -31,53 +31,60 @@
     <t>Código Python</t>
   </si>
   <si>
+    <t>Condición Python</t>
+  </si>
+  <si>
+    <t>Condición basada en</t>
+  </si>
+  <si>
     <t>Reglas (2)</t>
   </si>
   <si>
     <t>IGSS</t>
   </si>
   <si>
-    <t>001</t>
+    <t>B001</t>
   </si>
   <si>
     <t>Deducción</t>
   </si>
   <si>
+    <t>result = -(contract.wage - 250) * 0.0483</t>
+  </si>
+  <si>
     <t xml:space="preserve">
-                    # Available variables:
-                    #----------------------
-                    # payslip: object containing the payslips
-                    # employee: hr.employee object
-                    # contract: hr.contract object
-                    # rules: object containing the rules code (previously computed)
-                    # categories: object containing the computed salary rule categories (sum of amount of all rules belonging to that category).
-                    # worked_days: object containing the computed worked days.
-                    # inputs: object containing the computed inputs.
-                    # Note: returned value have to be set in the variable 'result'
-                    result = -(contract.wage - 250) * 0.0483</t>
+# Available variables:
+#----------------------
+# payslip: object containing the payslips
+# employee: hr.employee object
+# contract: hr.contract object
+# rules: object containing the rules code (previously computed)
+# categories: object containing the computed salary rule categories (sum of amount of all rules belonging to that category).
+# worked_days: object containing the computed worked days
+# inputs: object containing the computed inputs.
+# Note: returned value have to be set in the variable 'result'
+result = rules.NET &gt; categories.NET * 0.10</t>
+  </si>
+  <si>
+    <t>Siempre verdadero</t>
   </si>
   <si>
     <t>Horas extras</t>
   </si>
   <si>
-    <t>002</t>
+    <t>EXTRA_HOURS</t>
   </si>
   <si>
     <t>Básico</t>
   </si>
   <si>
-    <t xml:space="preserve">
-                    # Available variables:
-                    #----------------------
-                    # payslip: object containing the payslips
-                    # employee: hr.employee object
-                    # contract: hr.contract object
-                    # rules: object containing the rules code (previously computed)
-                    # categories: object containing the computed salary rule categories (sum of amount of all rules belonging to that category).
-                    # worked_days: object containing the computed worked days.
-                    # inputs: object containing the computed inputs.
-                    # Note: returned value have to be set in the variable 'result'
-                    result = contract.wage * 0.015</t>
+    <t>result = (contract.wage / 30 / 8) * 1.5  * inputs.EXTRA_HOURS.amount</t>
+  </si>
+  <si>
+    <t>result = inputs.EXTRA_HOURS</t>
+  </si>
+  <si>
+    <t>Expresión Python</t>
   </si>
 </sst>
 </file>
@@ -430,16 +437,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="30.7109375" customWidth="1"/>
+    <col min="1" max="7" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,48 +462,68 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>